<commit_message>
update value boxes and tables
</commit_message>
<xml_diff>
--- a/data-raw/district_summary.xlsx
+++ b/data-raw/district_summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Robinson/Afenet-projects/afenet-uganda/malariaRA/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABFF8A94-A5F8-6643-9777-0C8A0C6E63D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60E4EA9E-77B5-E04D-B7DC-1B89417CEADF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="13980" xr2:uid="{34179EBF-EA7A-454E-A815-C1EFFB15E6B7}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="13880" xr2:uid="{34179EBF-EA7A-454E-A815-C1EFFB15E6B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -412,7 +412,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>